<commit_message>
Mise à jour Planification.xlsx. Création Objectifs.docx (à compléter par tout le monde). Création Roles.docx qui défini les rôles de chaque participant.
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Planification</t>
   </si>
@@ -97,13 +97,7 @@
     <t>Rapport intérmédiaire</t>
   </si>
   <si>
-    <t>Fin rapport</t>
-  </si>
-  <si>
     <t>Préparation présentation</t>
-  </si>
-  <si>
-    <t>Fin 1ere it</t>
   </si>
 </sst>
 </file>
@@ -567,7 +561,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -683,48 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
@@ -759,6 +711,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1061,7 +1049,7 @@
   <dimension ref="A1:AZ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1072,120 +1060,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48">
+      <c r="B1" s="55">
         <v>8</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="47">
+      <c r="C1" s="56"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="54">
         <v>9</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="47">
+      <c r="G1" s="56"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="54">
         <v>10</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="47">
+      <c r="K1" s="56"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="54">
         <v>11</v>
       </c>
-      <c r="O1" s="48"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="47">
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="54">
         <v>12</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="47">
+      <c r="S1" s="55"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="54">
         <v>13</v>
       </c>
-      <c r="W1" s="48"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="47">
+      <c r="W1" s="55"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="54">
         <v>14</v>
       </c>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="47">
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="54">
         <v>15</v>
       </c>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="49"/>
-      <c r="AG1" s="50"/>
-      <c r="AH1" s="47">
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="54">
         <v>16</v>
       </c>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="51"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="57"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43">
+      <c r="A2" s="65"/>
+      <c r="B2" s="63">
         <v>40284</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="40" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="40" t="s">
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="46" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="46" t="s">
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="46" t="s">
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="46" t="s">
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="46" t="s">
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="46" t="s">
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60"/>
+      <c r="AH2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="41"/>
-      <c r="AK2" s="42"/>
+      <c r="AI2" s="59"/>
+      <c r="AJ2" s="59"/>
+      <c r="AK2" s="60"/>
     </row>
     <row r="3" spans="1:37" ht="23.25" customHeight="1">
       <c r="A3" s="18" t="s">
@@ -1194,11 +1182,11 @@
       <c r="B3" s="27"/>
       <c r="C3" s="15"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="56"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="33"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="61"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="33"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1235,7 +1223,7 @@
       <c r="B4" s="28"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="57"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="28"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1243,7 +1231,7 @@
       <c r="J4" s="28"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="55"/>
+      <c r="M4" s="41"/>
       <c r="N4" s="28"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -1276,7 +1264,7 @@
       <c r="B5" s="28"/>
       <c r="C5" s="5"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="58"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="28"/>
       <c r="G5" s="5"/>
       <c r="H5" s="17"/>
@@ -1317,10 +1305,10 @@
       <c r="B6" s="28"/>
       <c r="C6" s="5"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="28"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="62"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="6"/>
       <c r="J6" s="28"/>
       <c r="K6" s="5"/>
@@ -1355,10 +1343,10 @@
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="63"/>
+      <c r="B7" s="40"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
@@ -1395,9 +1383,10 @@
       <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="30"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1438,8 +1427,8 @@
       <c r="B9" s="28"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="64"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="50"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
@@ -1479,7 +1468,7 @@
       <c r="B10" s="28"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="58"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="30"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1520,9 +1509,9 @@
       <c r="B11" s="28"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="28"/>
@@ -1561,8 +1550,8 @@
       <c r="B12" s="28"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="67"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
@@ -1597,12 +1586,12 @@
     </row>
     <row r="13" spans="1:37" ht="23.25" customHeight="1">
       <c r="A13" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="58"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="28"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1641,7 +1630,7 @@
       <c r="B14" s="28"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="58"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="28"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1682,7 +1671,7 @@
       <c r="B15" s="28"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="58"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="28"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1723,7 +1712,7 @@
       <c r="B16" s="31"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="59"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="30"/>
       <c r="G16" s="34"/>
       <c r="H16" s="17"/>
@@ -1764,7 +1753,7 @@
       <c r="B17" s="23"/>
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
-      <c r="E17" s="60"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="23"/>
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
@@ -1920,9 +1909,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1978,9 +1965,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -2154,12 +2139,6 @@
     <row r="39" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A1:A2"/>
@@ -2173,6 +2152,12 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="J1:M1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Changement Rapport intermediaire.doc les diagrammes et Planification.xls sont mis en annexes. C'est plus facile s'il y a des modifications ensuite
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -88,9 +88,6 @@
     <t>Base de données</t>
   </si>
   <si>
-    <t>Gestion réseau</t>
-  </si>
-  <si>
     <t>Storry board</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>Préparation présentation</t>
+  </si>
+  <si>
+    <t>Gestion réseau et serveur</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -700,27 +700,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,27 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1052,7 +1040,7 @@
   <dimension ref="A1:AZ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO12" sqref="AO12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1063,120 +1051,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="62">
+      <c r="B1" s="52">
         <v>8</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="61">
+      <c r="C1" s="53"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="51">
         <v>9</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="61">
+      <c r="G1" s="53"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="51">
         <v>10</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="61">
+      <c r="K1" s="53"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="51">
         <v>11</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="61">
+      <c r="O1" s="52"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="51">
         <v>12</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="61">
+      <c r="S1" s="52"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="51">
         <v>13</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="61">
+      <c r="W1" s="52"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="51">
         <v>14</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="61">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="51">
         <v>15</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="61">
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="51">
         <v>16</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="65"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="54"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="59"/>
-      <c r="B2" s="57">
+      <c r="A2" s="62"/>
+      <c r="B2" s="60">
         <v>40284</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="54" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="54" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="60" t="s">
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="60" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="60" t="s">
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="60" t="s">
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="60" t="s">
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="60" t="s">
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="56"/>
+      <c r="AI2" s="56"/>
+      <c r="AJ2" s="56"/>
+      <c r="AK2" s="57"/>
     </row>
     <row r="3" spans="1:37" ht="23.25" customHeight="1">
       <c r="A3" s="18" t="s">
@@ -1221,7 +1209,7 @@
     </row>
     <row r="4" spans="1:37" ht="23.25" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="5"/>
@@ -1346,7 +1334,8 @@
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="24"/>
       <c r="E7" s="45"/>
       <c r="F7" s="49"/>
@@ -1384,7 +1373,7 @@
     </row>
     <row r="8" spans="1:37" ht="23.25" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="48"/>
@@ -1395,7 +1384,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="52"/>
+      <c r="K8" s="50"/>
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
       <c r="N8" s="28"/>
@@ -1425,15 +1414,15 @@
     </row>
     <row r="9" spans="1:37" ht="23.25" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="44"/>
-      <c r="F9" s="50"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="6"/>
       <c r="J9" s="28"/>
       <c r="K9" s="5"/>
@@ -1476,8 +1465,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="30"/>
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
       <c r="N10" s="28"/>
@@ -1513,30 +1501,20 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="44"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="F11" s="30"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="66"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="52"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="28"/>
-      <c r="AA11" s="52"/>
-      <c r="AB11" s="66"/>
-      <c r="AC11" s="6"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="30"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="30"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="30"/>
+      <c r="AC11" s="29"/>
       <c r="AD11" s="28"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
@@ -1554,7 +1532,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="44"/>
-      <c r="F12" s="53"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
@@ -1589,7 +1567,7 @@
     </row>
     <row r="13" spans="1:37" ht="23.25" customHeight="1">
       <c r="A13" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="5"/>
@@ -1623,10 +1601,10 @@
       <c r="AE13" s="34"/>
       <c r="AF13" s="17"/>
       <c r="AG13" s="29"/>
-      <c r="AH13" s="35"/>
-      <c r="AI13" s="36"/>
-      <c r="AJ13" s="37"/>
-      <c r="AK13" s="38"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="34"/>
+      <c r="AJ13" s="17"/>
+      <c r="AK13" s="29"/>
     </row>
     <row r="14" spans="1:37" ht="23.25" customHeight="1">
       <c r="A14" s="14"/>
@@ -2142,12 +2120,6 @@
     <row r="39" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A1:A2"/>
@@ -2161,9 +2133,15 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="J1:M1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="R3:AK12">
+  <conditionalFormatting sqref="AD3:AK12 R3:AC10 R12:AC12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="f"/>
@@ -2173,7 +2151,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:AK12">
+  <conditionalFormatting sqref="AD3:AK12 V3:AC10 V12:AC12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
Itérations mis à jour en fonctions des remarques
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="-225" windowWidth="21840" windowHeight="13350"/>
+    <workbookView xWindow="435" yWindow="-225" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -548,6 +548,17 @@
       <top style="hair">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -561,7 +572,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -703,6 +714,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,32 +744,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1039,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1051,120 +1065,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="52">
+      <c r="B1" s="59">
         <v>8</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="51">
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="58">
         <v>9</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="51">
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="58">
         <v>10</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="51">
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="58">
         <v>11</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="51">
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="58">
         <v>12</v>
       </c>
-      <c r="S1" s="52"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="51">
+      <c r="S1" s="59"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="58">
         <v>13</v>
       </c>
-      <c r="W1" s="52"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="51">
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="58">
         <v>14</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="51">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="58">
         <v>15</v>
       </c>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="51">
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="60"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="58">
         <v>16</v>
       </c>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="54"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="60"/>
+      <c r="AK1" s="62"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="62"/>
-      <c r="B2" s="60">
+      <c r="A2" s="56"/>
+      <c r="B2" s="54">
         <v>40284</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="59" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="59" t="s">
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="55" t="s">
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="55" t="s">
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="55" t="s">
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="55" t="s">
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="55" t="s">
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="57"/>
-      <c r="AH2" s="55" t="s">
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="57"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="53"/>
     </row>
     <row r="3" spans="1:37" ht="23.25" customHeight="1">
       <c r="A3" s="18" t="s">
@@ -1226,7 +1240,7 @@
       <c r="N4" s="28"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="6"/>
+      <c r="Q4" s="41"/>
       <c r="R4" s="28"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -1265,7 +1279,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
       <c r="N5" s="28"/>
-      <c r="O5" s="5"/>
+      <c r="O5" s="17"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="28"/>
@@ -1347,7 +1361,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="6"/>
       <c r="N7" s="28"/>
-      <c r="O7" s="5"/>
+      <c r="O7" s="34"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="28"/>
@@ -1388,7 +1402,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="5"/>
+      <c r="O8" s="50"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="28"/>
@@ -1438,11 +1452,11 @@
       <c r="U9" s="6"/>
       <c r="V9" s="28"/>
       <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
+      <c r="X9" s="17"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="28"/>
       <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
+      <c r="AB9" s="17"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="28"/>
       <c r="AE9" s="5"/>
@@ -1515,10 +1529,8 @@
       <c r="Y11" s="29"/>
       <c r="Z11" s="30"/>
       <c r="AC11" s="29"/>
-      <c r="AD11" s="28"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="6"/>
+      <c r="AD11" s="30"/>
+      <c r="AG11" s="29"/>
       <c r="AH11" s="8"/>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
@@ -1597,10 +1609,10 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="6"/>
-      <c r="AD13" s="30"/>
+      <c r="AD13" s="28"/>
       <c r="AE13" s="34"/>
       <c r="AF13" s="17"/>
-      <c r="AG13" s="29"/>
+      <c r="AG13" s="6"/>
       <c r="AH13" s="30"/>
       <c r="AI13" s="34"/>
       <c r="AJ13" s="17"/>
@@ -1636,10 +1648,10 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="6"/>
-      <c r="AD14" s="28"/>
+      <c r="AD14" s="30"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
-      <c r="AG14" s="6"/>
+      <c r="AG14" s="29"/>
       <c r="AH14" s="8"/>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
@@ -1758,12 +1770,12 @@
       <c r="Z17" s="23"/>
       <c r="AA17" s="25"/>
       <c r="AB17" s="26"/>
-      <c r="AC17" s="32"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="37"/>
-      <c r="AG17" s="38"/>
-      <c r="AH17" s="35"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="32"/>
+      <c r="AH17" s="63"/>
       <c r="AI17" s="36"/>
       <c r="AJ17" s="37"/>
       <c r="AK17" s="38"/>
@@ -2078,10 +2090,8 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
-      <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
@@ -2120,6 +2130,12 @@
     <row r="39" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A1:A2"/>
@@ -2133,15 +2149,9 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="J1:M1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="AD3:AK12 R3:AC10 R12:AC12">
+  <conditionalFormatting sqref="AH3:AK12 R3:AG10 R12:AG12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="f"/>
@@ -2151,7 +2161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD3:AK12 V3:AC10 V12:AC12">
+  <conditionalFormatting sqref="AH3:AK12 V3:AG10 V12:AG12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>